<commit_message>
[#57750402] working on author coinstitution networks
Need to work on the networks.py to define nodes properly from readers.


Former-commit-id: 7f23d43be79241fb3f2cbc16b90e3baefb37323f
</commit_message>
<xml_diff>
--- a/tethne/testsuite/TestCases_Modules_status.xlsx
+++ b/tethne/testsuite/TestCases_Modules_status.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="72" windowWidth="15300" windowHeight="6360"/>
+    <workbookView xWindow="100" yWindow="80" windowWidth="15300" windowHeight="6360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="author coinstitutions" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="99">
   <si>
     <t>Module Name</t>
   </si>
@@ -253,13 +258,73 @@
   </si>
   <si>
     <t>writers_test.py</t>
+  </si>
+  <si>
+    <t>C1 [Galar, Mike; Barrenechea, Edurne] Univ Publ Navarra, Dept Automat &amp; Comp, Pamplona 31006, Spain.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [Fernandez, Alberto] Univ Jaen, Dept Comp Sci, Jaen 23071, Spain.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   [Herrera, Francisco] Univ Granada, Dept Comp Sci &amp; Artificial Intelligence, E-18071 Granada, Spain.</t>
+  </si>
+  <si>
+    <t>C1 United Arab Emirates Univ, Dept Architectural Engn, Al Ain, U Arab Emirates.</t>
+  </si>
+  <si>
+    <t>author with Initials</t>
+  </si>
+  <si>
+    <t>author with full names</t>
+  </si>
+  <si>
+    <t>paper 1</t>
+  </si>
+  <si>
+    <t>paper 2</t>
+  </si>
+  <si>
+    <t>paper 3</t>
+  </si>
+  <si>
+    <t>Author coinstitutions : Input forms - 3 types</t>
+  </si>
+  <si>
+    <t>C1 - field corresponds to this.</t>
+  </si>
+  <si>
+    <t>no author affliations</t>
+  </si>
+  <si>
+    <t>authors are</t>
+  </si>
+  <si>
+    <t>AF Elsheshtawy, Yasser</t>
+  </si>
+  <si>
+    <t>C1 [Chen, T. Y.; Huang, J. H.] Univ Granada, Dept Comp Sci &amp; Artificial Intelligence, E-18071 Granada, Spain</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>C1 Field</t>
+  </si>
+  <si>
+    <t>paper ID</t>
+  </si>
+  <si>
+    <t>NetworkX Graph will be</t>
+  </si>
+  <si>
+    <t>Similarily Galar and Barraenechea (of papers 1) share Univ of Publ Navarra with each</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,8 +340,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,6 +375,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -300,35 +393,50 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -351,8 +459,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="16">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,6 +557,472 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3669452</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>164254</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4868333</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>98214</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Connector 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4346785" y="3737187"/>
+          <a:ext cx="1198881" cy="822960"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Univ of</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0"/>
+            <a:t> Granada</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2590800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>42334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3479801</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>143934</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Connector 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3268133" y="5215467"/>
+          <a:ext cx="889001" cy="635000"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Herrera(P1)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4524588</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>88053</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5347548</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>22013</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5201921" y="4549986"/>
+          <a:ext cx="822960" cy="822960"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3877734</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>67735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4690534</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>8467</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Connector 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4555067" y="5240868"/>
+          <a:ext cx="812800" cy="651932"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Chen T (P3)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5080000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>118532</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5935134</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>25399</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Connector 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5757333" y="5291665"/>
+          <a:ext cx="855134" cy="618067"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Huang JH (P3)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4343400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>16934</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4463626</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>145627</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Connector 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5020733" y="4656667"/>
+          <a:ext cx="120226" cy="662093"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2770294</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3733801</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>154093</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3447627" y="4512733"/>
+          <a:ext cx="963507" cy="636693"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle" w="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3479801</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>4234</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3877734</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Connector 13"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="6"/>
+          <a:endCxn id="6" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4157134" y="5532967"/>
+          <a:ext cx="397933" cy="33867"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4690534</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5088467</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>122767</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Connector 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5367867" y="5617633"/>
+          <a:ext cx="397933" cy="33867"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -441,7 +1031,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFBF0"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -722,24 +1312,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I18" sqref="I18"/>
+      <selection pane="topRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.5" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -768,7 +1358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -797,7 +1387,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -826,7 +1416,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -855,7 +1445,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -884,7 +1474,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -913,7 +1503,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -942,7 +1532,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -971,7 +1561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1000,7 +1590,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -1029,7 +1619,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -1058,7 +1648,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -1087,7 +1677,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" s="7">
         <v>12</v>
       </c>
@@ -1116,7 +1706,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -1145,7 +1735,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" s="7">
         <v>14</v>
       </c>
@@ -1174,7 +1764,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -1203,7 +1793,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18" s="7">
         <v>16</v>
       </c>
@@ -1232,7 +1822,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20" s="7">
         <v>17</v>
       </c>
@@ -1261,7 +1851,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9">
       <c r="A21" s="7">
         <v>18</v>
       </c>
@@ -1290,7 +1880,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22" s="7">
         <v>19</v>
       </c>
@@ -1319,7 +1909,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -1348,7 +1938,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="7">
         <v>21</v>
       </c>
@@ -1379,21 +1969,181 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15">
+      <c r="A4" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1403,8 +2153,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[#60216304] test-scripts for author institutions parsing - readers
committing till what has been completed. to continue on the unfinished
work.


Former-commit-id: 2d74fc10e0c7879264162b497add37c5173a1e55
</commit_message>
<xml_diff>
--- a/tethne/testsuite/TestCases_Modules_status.xlsx
+++ b/tethne/testsuite/TestCases_Modules_status.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="80" windowWidth="15300" windowHeight="6360" activeTab="1"/>
+    <workbookView xWindow="3980" yWindow="3300" windowWidth="15300" windowHeight="6360" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="author coinstitutions" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="test cases for auhor institutio" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="142">
   <si>
     <t>Module Name</t>
   </si>
@@ -317,14 +317,143 @@
     <t>NetworkX Graph will be</t>
   </si>
   <si>
-    <t>Similarily Galar and Barraenechea (of papers 1) share Univ of Publ Navarra with each</t>
+    <t>Cases to be checked</t>
+  </si>
+  <si>
+    <t>5 authors in AF field, only 2 authors are affliated to institutions in C1 field</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Arrived</t>
+  </si>
+  <si>
+    <t>Status of test case</t>
+  </si>
+  <si>
+    <t>whether Last Name of author is in UPPER CASE of Output field</t>
+  </si>
+  <si>
+    <t>N authors in AU field but N-2 institutions in C1 field</t>
+  </si>
+  <si>
+    <t>whether First Name of author is in UPPER CASE of Output field</t>
+  </si>
+  <si>
+    <t>Example input</t>
+  </si>
+  <si>
+    <t>Example Output</t>
+  </si>
+  <si>
+    <t>Exception?</t>
+  </si>
+  <si>
+    <t>Code Change required?</t>
+  </si>
+  <si>
+    <t>C1 field</t>
+  </si>
+  <si>
+    <t>C1 field with No authors</t>
+  </si>
+  <si>
+    <t>C1 field with 1 mapping of author : inst</t>
+  </si>
+  <si>
+    <t>C1 field with 2 hetrogenous mappings of author : inst</t>
+  </si>
+  <si>
+    <t>C1 field with 2 homo genous mappings of author : inst</t>
+  </si>
+  <si>
+    <t>C1 field with 5 hetrogenous mappings of author : inst</t>
+  </si>
+  <si>
+    <t>C1 field with 3 homogenous and 2 hetrogenous mappings of author : inst</t>
+  </si>
+  <si>
+    <t>C1 field with No authors but without comma seperators</t>
+  </si>
+  <si>
+    <t>C1 field with No authors but with ; delimitors instead of ,</t>
+  </si>
+  <si>
+    <t>C1 field with 2 authors but with , delimitors instead of ;</t>
+  </si>
+  <si>
+    <t>C1 field and AU field combo</t>
+  </si>
+  <si>
+    <t>C1 field with 2 authors but with [ ] are missing</t>
+  </si>
+  <si>
+    <t>C1 field with 2 institutions in 2 different lines but no specific author affliations</t>
+  </si>
+  <si>
+    <t>3 authors in AF field, no authors are affliated to institutions in C1 field</t>
+  </si>
+  <si>
+    <t>File with only one record</t>
+  </si>
+  <si>
+    <t>File with only 2 records</t>
+  </si>
+  <si>
+    <t>File with no C1 field at all</t>
+  </si>
+  <si>
+    <t>Key Error exception of C1 field</t>
+  </si>
+  <si>
+    <t>File Level</t>
+  </si>
+  <si>
+    <t>AU and AF are not in sync, what will be the Output insitutions field?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Institutions field is 'None'</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Goes to the catch block if the author is already not present in the dict</t>
+  </si>
+  <si>
+    <t>UnboundLocalError: local variable 'wos_dict' referenced before assignment</t>
+  </si>
+  <si>
+    <t>No effect</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Pass - to be noted</t>
+  </si>
+  <si>
+    <t>ValueError: 'Lu, Chenglang' is not in list</t>
+  </si>
+  <si>
+    <t>ValueError: 'Wu, Zongda, Lu, Chenglang' is not in list</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,6 +488,20 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -418,7 +561,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -435,8 +578,40 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -460,8 +635,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="48">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -469,6 +652,22 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -477,6 +676,22 @@
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -929,97 +1144,6 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3479801</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>4234</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3877734</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Straight Connector 13"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="4" idx="6"/>
-          <a:endCxn id="6" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4157134" y="5532967"/>
-          <a:ext cx="397933" cy="33867"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4690534</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5088467</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>122767</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Straight Connector 15"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5367867" y="5617633"/>
-          <a:ext cx="397933" cy="33867"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1980,10 +2104,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D24"/>
+  <dimension ref="A2:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2128,11 +2252,6 @@
     <row r="23" spans="1:4">
       <c r="B23" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="C24" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2149,13 +2268,494 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="2" ySplit="15" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="60.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" customWidth="1"/>
+    <col min="7" max="7" width="32.1640625" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1"/>
+      <c r="B3" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1"/>
+      <c r="B10" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="1">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1">
+        <v>16</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" ht="42">
+      <c r="A22" s="8">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1"/>
+      <c r="B23" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" ht="42">
+      <c r="A24" s="1">
+        <v>19</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1">
+        <v>21</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>